<commit_message>
Page Folder Added in Cypress e2e folder and added login,mpin Test cases
</commit_message>
<xml_diff>
--- a/cypress/fixtures/PersonalDetailsVoterID.xlsx
+++ b/cypress/fixtures/PersonalDetailsVoterID.xlsx
@@ -89,10 +89,10 @@
     <t xml:space="preserve">spouseName</t>
   </si>
   <si>
+    <t xml:space="preserve">Raniji</t>
+  </si>
+  <si>
     <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
   </si>
   <si>
     <t xml:space="preserve">dob</t>
@@ -371,8 +371,8 @@
   </sheetPr>
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -491,15 +491,15 @@
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">

</xml_diff>